<commit_message>
test student , regression lineaire
</commit_message>
<xml_diff>
--- a/data/etho_tp2.xlsx
+++ b/data/etho_tp2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ellap\VirtualBox VMs\SciViews Box 2019\shared\projects\Ethologie-bourdons\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60E427A8-D694-4D8D-A0F1-3EB9D21CAE4C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F219C013-FEC5-4881-919E-802F2C1CD137}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{46521C02-9B3C-412F-B494-5CC5A24EFC83}"/>
   </bookViews>
@@ -31,36 +31,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="7">
   <si>
     <t>Individu</t>
-  </si>
-  <si>
-    <t>0 ,28</t>
-  </si>
-  <si>
-    <t>0 ,24</t>
-  </si>
-  <si>
-    <t>0 ,32</t>
-  </si>
-  <si>
-    <t>0,3à</t>
-  </si>
-  <si>
-    <t>0,2§</t>
-  </si>
-  <si>
-    <t>3 ,5</t>
-  </si>
-  <si>
-    <t>3 ,6</t>
-  </si>
-  <si>
-    <t>3 ,1</t>
-  </si>
-  <si>
-    <t>2 ,9</t>
   </si>
   <si>
     <t>sexe</t>
@@ -432,8 +405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E115C2CD-8B53-482C-B7D5-F04BA8322A05}">
   <dimension ref="A2:E177"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E164" sqref="E164"/>
+    <sheetView tabSelected="1" topLeftCell="A152" workbookViewId="0">
+      <selection activeCell="B179" sqref="B179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -447,16 +420,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -473,7 +446,7 @@
         <v>4.5</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -490,7 +463,7 @@
         <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -507,7 +480,7 @@
         <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -524,7 +497,7 @@
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -541,7 +514,7 @@
         <v>3</v>
       </c>
       <c r="E7" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -558,7 +531,7 @@
         <v>3.1</v>
       </c>
       <c r="E8" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -575,7 +548,7 @@
         <v>3.2</v>
       </c>
       <c r="E9" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -592,7 +565,7 @@
         <v>3.5</v>
       </c>
       <c r="E10" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -609,7 +582,7 @@
         <v>4</v>
       </c>
       <c r="E11" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -626,7 +599,7 @@
         <v>3.2</v>
       </c>
       <c r="E12" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -643,7 +616,7 @@
         <v>4</v>
       </c>
       <c r="E13" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -660,7 +633,7 @@
         <v>3</v>
       </c>
       <c r="E14" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -677,7 +650,7 @@
         <v>3.8</v>
       </c>
       <c r="E15" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -694,7 +667,7 @@
         <v>3</v>
       </c>
       <c r="E16" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -711,7 +684,7 @@
         <v>3</v>
       </c>
       <c r="E17" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -728,7 +701,7 @@
         <v>3.5</v>
       </c>
       <c r="E18" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -745,7 +718,7 @@
         <v>4</v>
       </c>
       <c r="E19" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -762,7 +735,7 @@
         <v>3.2</v>
       </c>
       <c r="E20" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -779,7 +752,7 @@
         <v>3</v>
       </c>
       <c r="E21" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -796,7 +769,7 @@
         <v>3.1</v>
       </c>
       <c r="E22" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -813,7 +786,7 @@
         <v>3.4</v>
       </c>
       <c r="E23" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -830,7 +803,7 @@
         <v>3.5</v>
       </c>
       <c r="E24" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -847,7 +820,7 @@
         <v>3.5</v>
       </c>
       <c r="E25" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -864,7 +837,7 @@
         <v>3.7</v>
       </c>
       <c r="E26" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -881,7 +854,7 @@
         <v>4</v>
       </c>
       <c r="E27" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -898,7 +871,7 @@
         <v>3.1</v>
       </c>
       <c r="E28" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
@@ -915,7 +888,7 @@
         <v>3</v>
       </c>
       <c r="E29" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
@@ -932,7 +905,7 @@
         <v>3.6</v>
       </c>
       <c r="E30" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -949,7 +922,7 @@
         <v>3.4</v>
       </c>
       <c r="E31" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
@@ -966,7 +939,7 @@
         <v>3.5</v>
       </c>
       <c r="E32" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
@@ -983,7 +956,7 @@
         <v>3.2</v>
       </c>
       <c r="E33" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
@@ -1000,7 +973,7 @@
         <v>3.6</v>
       </c>
       <c r="E34" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
@@ -1017,7 +990,7 @@
         <v>3</v>
       </c>
       <c r="E35" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
@@ -1034,7 +1007,7 @@
         <v>3.5</v>
       </c>
       <c r="E36" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
@@ -1051,7 +1024,7 @@
         <v>4</v>
       </c>
       <c r="E37" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
@@ -1064,11 +1037,11 @@
       <c r="C38">
         <v>15</v>
       </c>
-      <c r="D38" t="s">
-        <v>6</v>
+      <c r="D38">
+        <v>3.5</v>
       </c>
       <c r="E38" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
@@ -1085,7 +1058,7 @@
         <v>3.8</v>
       </c>
       <c r="E39" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
@@ -1102,7 +1075,7 @@
         <v>3</v>
       </c>
       <c r="E40" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
@@ -1119,7 +1092,7 @@
         <v>3.1</v>
       </c>
       <c r="E41" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
@@ -1136,7 +1109,7 @@
         <v>3.2</v>
       </c>
       <c r="E42" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
@@ -1153,15 +1126,15 @@
         <v>3</v>
       </c>
       <c r="E43" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>42</v>
       </c>
-      <c r="B44" t="s">
-        <v>1</v>
+      <c r="B44">
+        <v>0.28000000000000003</v>
       </c>
       <c r="C44">
         <v>14</v>
@@ -1170,7 +1143,7 @@
         <v>3.3</v>
       </c>
       <c r="E44" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
@@ -1187,7 +1160,7 @@
         <v>3.5</v>
       </c>
       <c r="E45" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
@@ -1204,7 +1177,7 @@
         <v>3</v>
       </c>
       <c r="E46" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
@@ -1221,7 +1194,7 @@
         <v>4.2</v>
       </c>
       <c r="E47" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
@@ -1238,7 +1211,7 @@
         <v>3.5</v>
       </c>
       <c r="E48" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -1255,7 +1228,7 @@
         <v>3</v>
       </c>
       <c r="E49" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
@@ -1272,7 +1245,7 @@
         <v>3.2</v>
       </c>
       <c r="E50" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
@@ -1289,7 +1262,7 @@
         <v>3</v>
       </c>
       <c r="E51" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
@@ -1306,7 +1279,7 @@
         <v>4</v>
       </c>
       <c r="E52" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
@@ -1323,7 +1296,7 @@
         <v>3.3</v>
       </c>
       <c r="E53" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
@@ -1340,7 +1313,7 @@
         <v>3.6</v>
       </c>
       <c r="E54" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
@@ -1357,7 +1330,7 @@
         <v>3.5</v>
       </c>
       <c r="E55" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
@@ -1374,7 +1347,7 @@
         <v>3.6</v>
       </c>
       <c r="E56" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
@@ -1391,7 +1364,7 @@
         <v>3.5</v>
       </c>
       <c r="E57" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
@@ -1408,7 +1381,7 @@
         <v>3.1</v>
       </c>
       <c r="E58" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
@@ -1425,7 +1398,7 @@
         <v>3.7</v>
       </c>
       <c r="E59" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
@@ -1442,7 +1415,7 @@
         <v>3.3</v>
       </c>
       <c r="E60" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
@@ -1459,7 +1432,7 @@
         <v>3</v>
       </c>
       <c r="E61" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
@@ -1476,7 +1449,7 @@
         <v>3.5</v>
       </c>
       <c r="E62" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
@@ -1493,7 +1466,7 @@
         <v>4</v>
       </c>
       <c r="E63" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
@@ -1510,7 +1483,7 @@
         <v>3.5</v>
       </c>
       <c r="E64" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
@@ -1527,7 +1500,7 @@
         <v>3.1</v>
       </c>
       <c r="E65" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
@@ -1544,7 +1517,7 @@
         <v>3.5</v>
       </c>
       <c r="E66" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
@@ -1561,7 +1534,7 @@
         <v>3</v>
       </c>
       <c r="E67" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
@@ -1578,7 +1551,7 @@
         <v>3.5</v>
       </c>
       <c r="E68" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
@@ -1595,7 +1568,7 @@
         <v>3</v>
       </c>
       <c r="E69" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
@@ -1612,7 +1585,7 @@
         <v>3.4</v>
       </c>
       <c r="E70" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
@@ -1629,7 +1602,7 @@
         <v>3.4</v>
       </c>
       <c r="E71" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
@@ -1646,7 +1619,7 @@
         <v>3</v>
       </c>
       <c r="E72" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
@@ -1663,7 +1636,7 @@
         <v>3</v>
       </c>
       <c r="E73" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
@@ -1680,7 +1653,7 @@
         <v>3</v>
       </c>
       <c r="E74" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
@@ -1697,7 +1670,7 @@
         <v>3.2</v>
       </c>
       <c r="E75" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
@@ -1714,7 +1687,7 @@
         <v>3.8</v>
       </c>
       <c r="E76" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
@@ -1731,7 +1704,7 @@
         <v>3.2</v>
       </c>
       <c r="E77" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
@@ -1748,7 +1721,7 @@
         <v>3</v>
       </c>
       <c r="E78" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
@@ -1765,7 +1738,7 @@
         <v>3.1</v>
       </c>
       <c r="E79" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
@@ -1782,7 +1755,7 @@
         <v>3</v>
       </c>
       <c r="E80" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
@@ -1799,15 +1772,15 @@
         <v>3</v>
       </c>
       <c r="E81" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>80</v>
       </c>
-      <c r="B82" t="s">
-        <v>2</v>
+      <c r="B82">
+        <v>0.24</v>
       </c>
       <c r="C82">
         <v>13</v>
@@ -1816,7 +1789,7 @@
         <v>3</v>
       </c>
       <c r="E82" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
@@ -1833,7 +1806,7 @@
         <v>3</v>
       </c>
       <c r="E83" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
@@ -1850,7 +1823,7 @@
         <v>3.5</v>
       </c>
       <c r="E84" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
@@ -1867,7 +1840,7 @@
         <v>4</v>
       </c>
       <c r="E85" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
@@ -1884,7 +1857,7 @@
         <v>3.1</v>
       </c>
       <c r="E86" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
@@ -1901,7 +1874,7 @@
         <v>3.3</v>
       </c>
       <c r="E87" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.3">
@@ -1918,7 +1891,7 @@
         <v>3.5</v>
       </c>
       <c r="E88" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
@@ -1935,7 +1908,7 @@
         <v>3</v>
       </c>
       <c r="E89" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
@@ -1952,7 +1925,7 @@
         <v>3.3</v>
       </c>
       <c r="E90" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
@@ -1969,7 +1942,7 @@
         <v>3.5</v>
       </c>
       <c r="E91" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
@@ -1986,7 +1959,7 @@
         <v>4</v>
       </c>
       <c r="E92" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.3">
@@ -2003,7 +1976,7 @@
         <v>4</v>
       </c>
       <c r="E93" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
@@ -2020,7 +1993,7 @@
         <v>2.8</v>
       </c>
       <c r="E94" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.3">
@@ -2037,7 +2010,7 @@
         <v>3.6</v>
       </c>
       <c r="E95" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.3">
@@ -2054,7 +2027,7 @@
         <v>3.5</v>
       </c>
       <c r="E96" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.3">
@@ -2071,7 +2044,7 @@
         <v>3</v>
       </c>
       <c r="E97" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.3">
@@ -2088,7 +2061,7 @@
         <v>3.7</v>
       </c>
       <c r="E98" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.3">
@@ -2105,7 +2078,7 @@
         <v>2.9</v>
       </c>
       <c r="E99" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.3">
@@ -2122,7 +2095,7 @@
         <v>3.8</v>
       </c>
       <c r="E100" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.3">
@@ -2139,15 +2112,15 @@
         <v>3.4</v>
       </c>
       <c r="E101" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>100</v>
       </c>
-      <c r="B102" t="s">
-        <v>3</v>
+      <c r="B102">
+        <v>0.32</v>
       </c>
       <c r="C102">
         <v>16</v>
@@ -2156,7 +2129,7 @@
         <v>3.5</v>
       </c>
       <c r="E102" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
@@ -2173,7 +2146,7 @@
         <v>2.9</v>
       </c>
       <c r="E103" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.3">
@@ -2186,11 +2159,11 @@
       <c r="C104">
         <v>15</v>
       </c>
-      <c r="D104" t="s">
-        <v>7</v>
+      <c r="D104">
+        <v>3.6</v>
       </c>
       <c r="E104" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
@@ -2207,7 +2180,7 @@
         <v>3</v>
       </c>
       <c r="E105" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.3">
@@ -2224,7 +2197,7 @@
         <v>3.3</v>
       </c>
       <c r="E106" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.3">
@@ -2241,7 +2214,7 @@
         <v>3</v>
       </c>
       <c r="E107" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
@@ -2258,7 +2231,7 @@
         <v>3.6</v>
       </c>
       <c r="E108" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.3">
@@ -2275,7 +2248,7 @@
         <v>3.1</v>
       </c>
       <c r="E109" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.3">
@@ -2292,7 +2265,7 @@
         <v>3.5</v>
       </c>
       <c r="E110" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.3">
@@ -2309,7 +2282,7 @@
         <v>3.3</v>
       </c>
       <c r="E111" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.3">
@@ -2326,7 +2299,7 @@
         <v>3.2</v>
       </c>
       <c r="E112" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.3">
@@ -2343,7 +2316,7 @@
         <v>3</v>
       </c>
       <c r="E113" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.3">
@@ -2356,11 +2329,11 @@
       <c r="C114">
         <v>14</v>
       </c>
-      <c r="D114" t="s">
-        <v>8</v>
+      <c r="D114">
+        <v>3.1</v>
       </c>
       <c r="E114" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.3">
@@ -2377,7 +2350,7 @@
         <v>3.6</v>
       </c>
       <c r="E115" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.3">
@@ -2394,7 +2367,7 @@
         <v>3.2</v>
       </c>
       <c r="E116" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.3">
@@ -2411,7 +2384,7 @@
         <v>3</v>
       </c>
       <c r="E117" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.3">
@@ -2428,7 +2401,7 @@
         <v>3.2</v>
       </c>
       <c r="E118" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.3">
@@ -2445,7 +2418,7 @@
         <v>3</v>
       </c>
       <c r="E119" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.3">
@@ -2462,7 +2435,7 @@
         <v>3</v>
       </c>
       <c r="E120" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.3">
@@ -2479,15 +2452,15 @@
         <v>3.1</v>
       </c>
       <c r="E121" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>120</v>
       </c>
-      <c r="B122" t="s">
-        <v>4</v>
+      <c r="B122">
+        <v>0.3</v>
       </c>
       <c r="C122">
         <v>15</v>
@@ -2496,7 +2469,7 @@
         <v>3.2</v>
       </c>
       <c r="E122" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.3">
@@ -2513,7 +2486,7 @@
         <v>2.6</v>
       </c>
       <c r="E123" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.3">
@@ -2530,7 +2503,7 @@
         <v>3.1</v>
       </c>
       <c r="E124" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.3">
@@ -2547,7 +2520,7 @@
         <v>3.5</v>
       </c>
       <c r="E125" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.3">
@@ -2564,7 +2537,7 @@
         <v>3.4</v>
       </c>
       <c r="E126" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.3">
@@ -2581,15 +2554,15 @@
         <v>3.2</v>
       </c>
       <c r="E127" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>126</v>
       </c>
-      <c r="B128" t="s">
-        <v>5</v>
+      <c r="B128">
+        <v>0.25</v>
       </c>
       <c r="C128">
         <v>15</v>
@@ -2598,7 +2571,7 @@
         <v>3</v>
       </c>
       <c r="E128" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.3">
@@ -2615,7 +2588,7 @@
         <v>3.5</v>
       </c>
       <c r="E129" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.3">
@@ -2632,7 +2605,7 @@
         <v>3</v>
       </c>
       <c r="E130" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.3">
@@ -2649,7 +2622,7 @@
         <v>3.4</v>
       </c>
       <c r="E131" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.3">
@@ -2666,7 +2639,7 @@
         <v>3</v>
       </c>
       <c r="E132" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.3">
@@ -2683,7 +2656,7 @@
         <v>3</v>
       </c>
       <c r="E133" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.3">
@@ -2700,7 +2673,7 @@
         <v>3.7</v>
       </c>
       <c r="E134" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.3">
@@ -2717,7 +2690,7 @@
         <v>3</v>
       </c>
       <c r="E135" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.3">
@@ -2734,7 +2707,7 @@
         <v>3.5</v>
       </c>
       <c r="E136" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.3">
@@ -2751,7 +2724,7 @@
         <v>3.1</v>
       </c>
       <c r="E137" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.3">
@@ -2768,7 +2741,7 @@
         <v>3.2</v>
       </c>
       <c r="E138" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.3">
@@ -2785,7 +2758,7 @@
         <v>3.2</v>
       </c>
       <c r="E139" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.3">
@@ -2802,7 +2775,7 @@
         <v>3.5</v>
       </c>
       <c r="E140" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.3">
@@ -2819,7 +2792,7 @@
         <v>3.6</v>
       </c>
       <c r="E141" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.3">
@@ -2836,7 +2809,7 @@
         <v>3</v>
       </c>
       <c r="E142" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.3">
@@ -2853,7 +2826,7 @@
         <v>2.9</v>
       </c>
       <c r="E143" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.3">
@@ -2870,7 +2843,7 @@
         <v>3.2</v>
       </c>
       <c r="E144" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.3">
@@ -2887,7 +2860,7 @@
         <v>3.1</v>
       </c>
       <c r="E145" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.3">
@@ -2900,11 +2873,11 @@
       <c r="C146">
         <v>13</v>
       </c>
-      <c r="D146" t="s">
-        <v>9</v>
+      <c r="D146">
+        <v>2.9</v>
       </c>
       <c r="E146" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.3">
@@ -2921,7 +2894,7 @@
         <v>3.1</v>
       </c>
       <c r="E147" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.3">
@@ -2938,7 +2911,7 @@
         <v>3</v>
       </c>
       <c r="E148" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.3">
@@ -2955,7 +2928,7 @@
         <v>3.5</v>
       </c>
       <c r="E149" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.3">
@@ -2972,7 +2945,7 @@
         <v>3</v>
       </c>
       <c r="E150" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.3">
@@ -2989,7 +2962,7 @@
         <v>3</v>
       </c>
       <c r="E151" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.3">
@@ -3006,7 +2979,7 @@
         <v>3.5</v>
       </c>
       <c r="E152" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.3">
@@ -3023,7 +2996,7 @@
         <v>4</v>
       </c>
       <c r="E153" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.3">
@@ -3040,7 +3013,7 @@
         <v>3.5</v>
       </c>
       <c r="E154" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.3">
@@ -3057,7 +3030,7 @@
         <v>3.2</v>
       </c>
       <c r="E155" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.3">
@@ -3074,7 +3047,7 @@
         <v>3.5</v>
       </c>
       <c r="E156" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.3">
@@ -3091,7 +3064,7 @@
         <v>3.1</v>
       </c>
       <c r="E157" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.3">
@@ -3099,7 +3072,7 @@
         <v>156</v>
       </c>
       <c r="B158">
-        <v>0.27850000000000003</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="C158">
         <v>13</v>
@@ -3108,7 +3081,7 @@
         <v>3</v>
       </c>
       <c r="E158" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.3">
@@ -3125,7 +3098,7 @@
         <v>3.3</v>
       </c>
       <c r="E159" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.3">
@@ -3142,7 +3115,7 @@
         <v>3.5</v>
       </c>
       <c r="E160" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.3">
@@ -3159,7 +3132,7 @@
         <v>3.2</v>
       </c>
       <c r="E161" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.3">
@@ -3176,7 +3149,7 @@
         <v>3.6</v>
       </c>
       <c r="E162" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.3">
@@ -3193,7 +3166,7 @@
         <v>3</v>
       </c>
       <c r="E163" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.3">
@@ -3210,15 +3183,15 @@
         <v>3.7</v>
       </c>
       <c r="E164" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>163</v>
       </c>
-      <c r="B165" t="s">
-        <v>4</v>
+      <c r="B165">
+        <v>0.3</v>
       </c>
       <c r="C165">
         <v>14</v>
@@ -3227,7 +3200,7 @@
         <v>3.5</v>
       </c>
       <c r="E165" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.3">
@@ -3244,7 +3217,7 @@
         <v>3.2</v>
       </c>
       <c r="E166" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.3">
@@ -3261,7 +3234,7 @@
         <v>3.4</v>
       </c>
       <c r="E167" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.3">
@@ -3278,7 +3251,7 @@
         <v>3.3</v>
       </c>
       <c r="E168" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.3">
@@ -3295,7 +3268,7 @@
         <v>2.8</v>
       </c>
       <c r="E169" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.3">
@@ -3312,7 +3285,7 @@
         <v>3.5</v>
       </c>
       <c r="E170" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.3">
@@ -3329,7 +3302,7 @@
         <v>3.5</v>
       </c>
       <c r="E171" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.3">
@@ -3346,7 +3319,7 @@
         <v>3.5</v>
       </c>
       <c r="E172" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.3">
@@ -3363,7 +3336,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="E173" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.3">
@@ -3380,7 +3353,7 @@
         <v>3.3</v>
       </c>
       <c r="E174" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.3">
@@ -3397,7 +3370,7 @@
         <v>2.7</v>
       </c>
       <c r="E175" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.3">
@@ -3414,7 +3387,7 @@
         <v>4.5</v>
       </c>
       <c r="E176" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.3">
@@ -3431,7 +3404,7 @@
         <v>3</v>
       </c>
       <c r="E177" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>